<commit_message>
Fixed BOM for E5 buddy board
</commit_message>
<xml_diff>
--- a/buddy/src/buddy_bom_rev1.xlsx
+++ b/buddy/src/buddy_bom_rev1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\All Customers\Adapteva\ND Jobs\ND2684-BUDDY Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aolofsson\Desktop\GIT\parallella-hw\buddy\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,39 +14,12 @@
   <sheets>
     <sheet name="BUDDY_SCH_JAN06_FINAL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
-  <si>
-    <t>Meta Connectors  Revised: Friday, January 06, 2017</t>
-  </si>
-  <si>
-    <t>Page content          Revision: 0</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>Bill Of Materials        January 6,2017      17:59:15</t>
-  </si>
-  <si>
-    <t>Page1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -63,15 +36,9 @@
     <t>Part Number</t>
   </si>
   <si>
-    <t>Part</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>______________________________________________</t>
-  </si>
-  <si>
     <t>C1,C2,C3,C4,C5,C6,C7,C8,C12,C13,C14,C15,C16,C17,C18,C19,C23,C24,C25,C26,C27,C28,C29,C30,C34,C35,C36,C37,C38,C39,C40,C41,C45,C46,C47,C48,C49,C50,C51,C52,C56,C57,C58,C59,C60,C61,C62,C63,C67,C68,C69,C70,C71,C72,C73,C74,C78,C79,C80,C81,C82,C83,C84,C85,C89,C90,C91,C92,C93,C94,C95,C96,C100,C101,C102,C103,C104,C105,C106,C107,C111,C112,C113,C114,C115,C116,C117,C118,C122,C123,C124,C125,C126,C127,C128,C129,C133,C134,C137,C138,C141,C142,C145,C146</t>
   </si>
   <si>
@@ -144,36 +111,9 @@
     <t>BGA Socket</t>
   </si>
   <si>
-    <t>R88,R103,R105,R106,R110,R111,R115,R116,R120,R121,R125,R126,R130,R131,R135,R136</t>
-  </si>
-  <si>
-    <t>VISHAY</t>
-  </si>
-  <si>
-    <t>CRCW04020000Z0ED</t>
-  </si>
-  <si>
-    <t>Resistor 0Ohm 1.5A 0402</t>
-  </si>
-  <si>
-    <t>R90,R101,R107,R108,R112,R113,R117,R118,R122,R123,R127,R128,R132,R133,R137,R138</t>
-  </si>
-  <si>
-    <t>PANASONIC CORP</t>
-  </si>
-  <si>
-    <t>ERJ-2RKF1000X</t>
-  </si>
-  <si>
-    <t>Resistor 100R 1/16W 1% SMD 0402</t>
-  </si>
-  <si>
     <t>R93,R94,R95,R96,R97,R98,R99,R100</t>
   </si>
   <si>
-    <t>Resistor 100R 1/10W 1% SMD 0402</t>
-  </si>
-  <si>
     <t>R102,R104,R109,R114,R119,R124,R129,R134</t>
   </si>
   <si>
@@ -184,13 +124,67 @@
   </si>
   <si>
     <t>E5</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>IRONWOOD</t>
+  </si>
+  <si>
+    <t>SG-BGA-6119</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>RC0402JR-070RL</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/16W 0402</t>
+  </si>
+  <si>
+    <t>R88,R103,R105,R106,R110,R111,R115,R116,R120,R121,R125,R126,R130,R131,R135,R136,R90,R101,R107,R108,R112,R113,R117,R118,R122,R123,R127,R128,R132,R133,R137,R138</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100RL</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>ADAPTEVA</t>
+  </si>
+  <si>
+    <t>AD0000</t>
+  </si>
+  <si>
+    <t>Epiphany-V Device</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,8 +319,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,8 +513,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -622,6 +635,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -667,8 +695,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -990,326 +1033,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
+      <c r="B2" s="4">
+        <v>104</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
+      <c r="B3" s="4">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
+      <c r="B4" s="4">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
+      <c r="B5" s="4">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
+      <c r="B6" s="4">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4">
+        <v>39299042</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B8" s="4">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
         <v>8</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="4">
+        <v>100</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B10" s="4">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
-        <v>15</v>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <f>SUM(B2:B11)</f>
+        <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>104</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19">
-        <v>39299042</v>
-      </c>
-      <c r="F19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8</v>
-      </c>
-      <c r="B22">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>9</v>
-      </c>
-      <c r="B23">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23">
-        <v>100</v>
-      </c>
-      <c r="G23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>10</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>11</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" t="s">
-        <v>54</v>
-      </c>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Adding updated buddy source files -Mostly manufacturing concerns -Schematic is still dirty, needs to be fixed. The BOM is correct.
</commit_message>
<xml_diff>
--- a/buddy/src/buddy_bom_rev1.xlsx
+++ b/buddy/src/buddy_bom_rev1.xlsx
@@ -1036,13 +1036,13 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>

</xml_diff>